<commit_message>
fix utils and maker
</commit_message>
<xml_diff>
--- a/base/Order_report/report.xlsx
+++ b/base/Order_report/report.xlsx
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +26,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="16"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDDDDD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -148,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -210,6 +219,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -553,10 +565,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:M22"/>
+  <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -567,10 +579,10 @@
     <col width="4.42578125" customWidth="1" style="10" min="6" max="6"/>
     <col width="42.28515625" customWidth="1" style="4" min="7" max="7"/>
     <col width="32.140625" customWidth="1" style="11" min="8" max="8"/>
-    <col width="15.140625" customWidth="1" style="11" min="9" max="10"/>
-    <col width="3.7109375" customWidth="1" min="11" max="11"/>
-    <col width="43.7109375" customWidth="1" min="12" max="12"/>
-    <col width="24" customWidth="1" min="13" max="13"/>
+    <col width="15.140625" customWidth="1" style="11" min="9" max="11"/>
+    <col width="3.7109375" customWidth="1" min="12" max="12"/>
+    <col width="43.7109375" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -589,14 +601,15 @@
       </c>
       <c r="H2" s="20" t="n"/>
       <c r="I2" s="20" t="n"/>
-      <c r="J2" s="21" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="19" t="inlineStr">
+      <c r="J2" s="20" t="n"/>
+      <c r="K2" s="21" t="n"/>
+      <c r="L2" s="3" t="n"/>
+      <c r="M2" s="19" t="inlineStr">
         <is>
           <t>Итог</t>
         </is>
       </c>
-      <c r="M2" s="21" t="n"/>
+      <c r="N2" s="21" t="n"/>
     </row>
     <row r="3">
       <c r="B3" s="22" t="n"/>
@@ -607,10 +620,11 @@
       <c r="G3" s="22" t="n"/>
       <c r="H3" s="23" t="n"/>
       <c r="I3" s="23" t="n"/>
-      <c r="J3" s="24" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="22" t="n"/>
-      <c r="M3" s="24" t="n"/>
+      <c r="J3" s="23" t="n"/>
+      <c r="K3" s="24" t="n"/>
+      <c r="L3" s="3" t="n"/>
+      <c r="M3" s="22" t="n"/>
+      <c r="N3" s="24" t="n"/>
     </row>
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
@@ -653,12 +667,17 @@
           <t>На сумму</t>
         </is>
       </c>
-      <c r="L4" s="6" t="inlineStr">
+      <c r="K4" s="18" t="inlineStr">
+        <is>
+          <t>Назначение</t>
+        </is>
+      </c>
+      <c r="M4" s="6" t="inlineStr">
         <is>
           <t>Компания:</t>
         </is>
       </c>
-      <c r="M4" s="1" t="inlineStr">
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>ТРК</t>
         </is>
@@ -685,21 +704,19 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G5" s="26" t="inlineStr">
+      <c r="G5" s="27" t="inlineStr">
         <is>
           <t>МЛРЗ</t>
         </is>
       </c>
-      <c r="H5" s="26" t="n"/>
-      <c r="I5" s="26" t="n"/>
-      <c r="L5" s="6" t="inlineStr">
+      <c r="M5" s="6" t="inlineStr">
         <is>
           <t>Указанный период:</t>
         </is>
       </c>
-      <c r="M5" s="1" t="inlineStr">
-        <is>
-          <t>2022-03-02 - 2022-03-24</t>
+      <c r="N5" s="1" t="inlineStr">
+        <is>
+          <t>2022-03-01 - 2022-03-25</t>
         </is>
       </c>
     </row>
@@ -724,28 +741,33 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G6" s="26" t="inlineStr">
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>33333</t>
         </is>
       </c>
-      <c r="H6" s="26" t="n">
+      <c r="H6" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="26" t="inlineStr">
+      <c r="I6" s="25" t="inlineStr">
         <is>
           <t>Чип-Дип</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="25" t="n">
         <v>132313</v>
       </c>
-      <c r="L6" s="6" t="inlineStr">
+      <c r="K6" s="25" t="inlineStr">
+        <is>
+          <t>Вагон 0555</t>
+        </is>
+      </c>
+      <c r="M6" s="6" t="inlineStr">
         <is>
           <t>Всего сформировано счетов:</t>
         </is>
       </c>
-      <c r="M6" s="1" t="n">
+      <c r="N6" s="1" t="n">
         <v>6</v>
       </c>
     </row>
@@ -770,28 +792,33 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G7" s="26" t="inlineStr">
+      <c r="G7" s="25" t="inlineStr">
         <is>
           <t>F44111</t>
         </is>
       </c>
-      <c r="H7" s="26" t="n">
+      <c r="H7" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="26" t="inlineStr">
+      <c r="I7" s="25" t="inlineStr">
         <is>
           <t>Чип-Дип</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="25" t="n">
         <v>2344</v>
       </c>
-      <c r="L7" s="6" t="inlineStr">
+      <c r="K7" s="25" t="inlineStr">
+        <is>
+          <t>УСИПУСИ</t>
+        </is>
+      </c>
+      <c r="M7" s="6" t="inlineStr">
         <is>
           <t>Общее количество заказанных компонентов:</t>
         </is>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="N7" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -818,20 +845,21 @@
       </c>
       <c r="G8" s="26" t="n"/>
       <c r="H8" s="26" t="n"/>
-      <c r="I8" s="26" t="inlineStr">
+      <c r="I8" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="25" t="n">
         <v>134657</v>
       </c>
-      <c r="L8" s="6" t="inlineStr">
+      <c r="K8" s="26" t="n"/>
+      <c r="M8" s="6" t="inlineStr">
         <is>
           <t>На сумму:</t>
         </is>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="N8" s="1" t="n">
         <v>709263</v>
       </c>
     </row>
@@ -856,15 +884,13 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G9" s="26" t="inlineStr">
+      <c r="G9" s="27" t="inlineStr">
         <is>
           <t>ИТЦСОиР</t>
         </is>
       </c>
-      <c r="H9" s="26" t="n"/>
-      <c r="I9" s="26" t="n"/>
-      <c r="L9" s="6" t="n"/>
-      <c r="M9" s="7" t="n"/>
+      <c r="M9" s="6" t="n"/>
+      <c r="N9" s="7" t="n"/>
     </row>
     <row r="10">
       <c r="B10" s="25" t="inlineStr">
@@ -887,28 +913,33 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G10" s="26" t="inlineStr">
+      <c r="G10" s="25" t="inlineStr">
         <is>
           <t>5487985A</t>
         </is>
       </c>
-      <c r="H10" s="26" t="n">
+      <c r="H10" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="I10" s="26" t="inlineStr">
+      <c r="I10" s="25" t="inlineStr">
         <is>
           <t>Элитан</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="25" t="n">
         <v>10000</v>
       </c>
-      <c r="L10" s="6" t="inlineStr">
+      <c r="K10" s="25" t="inlineStr">
+        <is>
+          <t>Ремонт</t>
+        </is>
+      </c>
+      <c r="M10" s="6" t="inlineStr">
         <is>
           <t>Самый маленький счет:</t>
         </is>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="N10" s="1" t="n">
         <v>2344</v>
       </c>
     </row>
@@ -933,28 +964,33 @@
           <t>12</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="25" t="inlineStr">
         <is>
           <t>133DD33</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="25" t="inlineStr">
         <is>
           <t>Чип-Дип</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="25" t="n">
         <v>34455</v>
       </c>
-      <c r="L11" s="6" t="inlineStr">
+      <c r="K11" s="25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M11" s="6" t="inlineStr">
         <is>
           <t>Самый большой счет:</t>
         </is>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="N11" s="1" t="n">
         <v>515151</v>
       </c>
     </row>
@@ -979,28 +1015,33 @@
           <t>13</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="25" t="inlineStr">
         <is>
           <t>555555</t>
         </is>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="25" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="25" t="n">
         <v>515151</v>
       </c>
-      <c r="L12" s="6" t="inlineStr">
+      <c r="K12" s="25" t="inlineStr">
+        <is>
+          <t>Ремонт</t>
+        </is>
+      </c>
+      <c r="M12" s="6" t="inlineStr">
         <is>
           <t>Средний счет:</t>
         </is>
       </c>
-      <c r="M12" s="1" t="n">
+      <c r="N12" s="1" t="n">
         <v>118210.5666666667</v>
       </c>
     </row>
@@ -1025,14 +1066,17 @@
           <t>25</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="G13" s="26" t="n"/>
+      <c r="H13" s="26" t="n"/>
+      <c r="I13" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="25" t="n">
         <v>559606</v>
       </c>
+      <c r="K13" s="26" t="n"/>
     </row>
     <row r="14">
       <c r="B14" s="25" t="inlineStr">
@@ -1055,97 +1099,119 @@
           <t>14</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="27" t="inlineStr">
         <is>
           <t>ИТЦ</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="I15" t="inlineStr">
+      <c r="G15" s="26" t="n"/>
+      <c r="H15" s="26" t="n"/>
+      <c r="I15" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="25" t="n">
         <v>0</v>
       </c>
+      <c r="K15" s="26" t="n"/>
     </row>
     <row r="16">
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="27" t="inlineStr">
         <is>
           <t>Ифыв</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="I17" t="inlineStr">
+      <c r="G17" s="26" t="n"/>
+      <c r="H17" s="26" t="n"/>
+      <c r="I17" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" s="25" t="n">
         <v>0</v>
       </c>
+      <c r="K17" s="26" t="n"/>
     </row>
     <row r="18">
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="27" t="inlineStr">
         <is>
           <t>Радиоцех</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="I19" t="inlineStr">
+      <c r="G19" s="26" t="n"/>
+      <c r="H19" s="26" t="n"/>
+      <c r="I19" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="25" t="n">
         <v>0</v>
       </c>
+      <c r="K19" s="26" t="n"/>
     </row>
     <row r="20">
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="27" t="inlineStr">
         <is>
           <t>ОРПВНП</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="G21" t="inlineStr">
+      <c r="G21" s="25" t="inlineStr">
         <is>
           <t>638608Z</t>
         </is>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" s="25" t="inlineStr">
         <is>
           <t>Чип-Дип</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="25" t="n">
         <v>15000.4</v>
       </c>
+      <c r="K21" s="25" t="inlineStr">
+        <is>
+          <t>Ремонт</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="I22" t="inlineStr">
+      <c r="G22" s="26" t="n"/>
+      <c r="H22" s="26" t="n"/>
+      <c r="I22" s="25" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="25" t="n">
         <v>15000.4</v>
       </c>
+      <c r="K22" s="26" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="L2:M3"/>
+  <mergeCells count="9">
+    <mergeCell ref="M2:N3"/>
     <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:J3"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G2:K3"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>

</xml_diff>